<commit_message>
Cap nhat he so 3p3z
</commit_message>
<xml_diff>
--- a/Cacheso2z2p.xlsx
+++ b/Cacheso2z2p.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="66">
   <si>
     <t>No</t>
   </si>
@@ -193,6 +193,30 @@
   </si>
   <si>
     <t>b3</t>
+  </si>
+  <si>
+    <t>Ít bị dính que hàn, dòng cao chưa ổn định</t>
+  </si>
+  <si>
+    <t>không bị dính que hàn, dòng cao chưa ổn định</t>
+  </si>
+  <si>
+    <t>Ít bị dính que hàn</t>
+  </si>
+  <si>
+    <t>hàn bị dính</t>
+  </si>
+  <si>
+    <t>để 30 thì bị dính</t>
+  </si>
+  <si>
+    <t>để 30 ít bị dính</t>
+  </si>
+  <si>
+    <t>dính, không được</t>
+  </si>
+  <si>
+    <t>để 30 đỡ dính hơn</t>
   </si>
 </sst>
 </file>
@@ -511,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI20"/>
+  <dimension ref="A1:AI33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1337,6 +1361,236 @@
         <v>3.3000000000000003E-5</v>
       </c>
     </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>180</v>
+      </c>
+      <c r="E22">
+        <v>16000</v>
+      </c>
+      <c r="F22">
+        <v>80000</v>
+      </c>
+      <c r="G22">
+        <v>1700</v>
+      </c>
+      <c r="H22">
+        <v>1700</v>
+      </c>
+      <c r="I22">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="K22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>1200</v>
+      </c>
+      <c r="E24">
+        <v>2200</v>
+      </c>
+      <c r="F24">
+        <v>80000</v>
+      </c>
+      <c r="G24">
+        <v>2600</v>
+      </c>
+      <c r="H24">
+        <v>16000</v>
+      </c>
+      <c r="I24">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>1200</v>
+      </c>
+      <c r="E26">
+        <v>2600</v>
+      </c>
+      <c r="F26">
+        <v>80000</v>
+      </c>
+      <c r="G26">
+        <v>2200</v>
+      </c>
+      <c r="H26">
+        <v>16000</v>
+      </c>
+      <c r="I26">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="K26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>1200</v>
+      </c>
+      <c r="E27">
+        <v>2600</v>
+      </c>
+      <c r="F27">
+        <v>40000</v>
+      </c>
+      <c r="G27">
+        <v>2200</v>
+      </c>
+      <c r="H27">
+        <v>16000</v>
+      </c>
+      <c r="I27">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="K27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>1200</v>
+      </c>
+      <c r="E28">
+        <v>2600</v>
+      </c>
+      <c r="F28">
+        <v>40000</v>
+      </c>
+      <c r="G28">
+        <v>2000</v>
+      </c>
+      <c r="H28">
+        <v>16000</v>
+      </c>
+      <c r="I28">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="K28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>1200</v>
+      </c>
+      <c r="E29">
+        <v>16000</v>
+      </c>
+      <c r="F29">
+        <v>40000</v>
+      </c>
+      <c r="G29">
+        <v>2600</v>
+      </c>
+      <c r="H29">
+        <v>3400</v>
+      </c>
+      <c r="I29">
+        <v>0.03</v>
+      </c>
+      <c r="K29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>800</v>
+      </c>
+      <c r="E30">
+        <v>16000</v>
+      </c>
+      <c r="F30">
+        <v>40000</v>
+      </c>
+      <c r="G30">
+        <v>2000</v>
+      </c>
+      <c r="H30">
+        <v>3400</v>
+      </c>
+      <c r="I30">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="K30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <v>800</v>
+      </c>
+      <c r="E31">
+        <v>16000</v>
+      </c>
+      <c r="F31">
+        <v>40000</v>
+      </c>
+      <c r="G31">
+        <v>1800</v>
+      </c>
+      <c r="H31">
+        <v>3800</v>
+      </c>
+      <c r="I31">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="K31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>700</v>
+      </c>
+      <c r="E32">
+        <v>16000</v>
+      </c>
+      <c r="F32">
+        <v>40000</v>
+      </c>
+      <c r="G32">
+        <v>1600</v>
+      </c>
+      <c r="H32">
+        <v>4000</v>
+      </c>
+      <c r="I32">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="K32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>800</v>
+      </c>
+      <c r="E33">
+        <v>20000</v>
+      </c>
+      <c r="F33">
+        <v>40000</v>
+      </c>
+      <c r="G33">
+        <v>1800</v>
+      </c>
+      <c r="H33">
+        <v>3800</v>
+      </c>
+      <c r="I33">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J33" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="K33" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="B2">
     <sortCondition ref="B2"/>

</xml_diff>